<commit_message>
updated base dmd for ship point state and new ootb dam model
</commit_message>
<xml_diff>
--- a/jcp-v4/99-exceldmd/Base Data Model.xlsx
+++ b/jcp-v4/99-exceldmd/Base Data Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shyam.potta/rdp-sourcecode/dataplatform-sampledata/jcp-dmd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/dataplatform-sampledata/jcp-v4/99-exceldmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="19640" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -45,8 +45,8 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -3902,12 +3902,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
+      <selection activeCell="A5" sqref="A5"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
       <selection activeCell="B34" sqref="B34"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
-      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4079,11 +4079,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4159,14 +4159,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4183,7 +4183,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8636,7 +8636,7 @@
         <v>160</v>
       </c>
       <c r="F141" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G141" t="s">
         <v>42</v>
@@ -8658,7 +8658,7 @@
         <v>160</v>
       </c>
       <c r="F142" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G142" t="s">
         <v>42</v>
@@ -11287,9 +11287,9 @@
   </sheetData>
   <autoFilter ref="A1:AE255"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11297,9 +11297,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11530,14 +11530,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -17044,12 +17044,6 @@
   </sheetData>
   <autoFilter ref="A1:AA475"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
-    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17060,6 +17054,12 @@
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D150">
@@ -17156,12 +17156,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17264,12 +17264,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17355,12 +17355,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed the format for DAM OOTB Data Model
</commit_message>
<xml_diff>
--- a/jcp-v4/99-exceldmd/Base Data Model.xlsx
+++ b/jcp-v4/99-exceldmd/Base Data Model.xlsx
@@ -43,10 +43,10 @@
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$459</definedName>
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -3902,12 +3902,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
+      <selection activeCell="B34" sqref="B34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
       <selection activeCell="A5" sqref="A5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
-      <selection activeCell="B34" sqref="B34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4079,11 +4079,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4159,14 +4159,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4180,10 +4180,10 @@
   <dimension ref="A1:AF255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11287,9 +11287,9 @@
   </sheetData>
   <autoFilter ref="A1:AE255"/>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11297,9 +11297,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11530,14 +11530,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -17044,6 +17044,12 @@
   </sheetData>
   <autoFilter ref="A1:AA475"/>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17054,12 +17060,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D150">
@@ -17156,12 +17156,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17264,12 +17264,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17355,12 +17355,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17372,6 +17372,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-24</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
+      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-24</Url>
+      <Description>Z7QZ4QWJDNQ7-73874190-24</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF273DB610BE64D8338C714685CCF46" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2352d1590348b4df6d1de565ccbd102a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fff5a07-2326-481b-a4e9-87ff7a79f8dd" xmlns:ns3="2e2046eb-f52d-433a-aad8-97c651e3992c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5c0a0cba47b5c64de8255dd546e4ec9" ns2:_="" ns3:_="">
     <xsd:import namespace="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
@@ -17549,7 +17561,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -17599,7 +17611,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17608,19 +17620,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-24</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
-      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-24</Url>
-      <Description>Z7QZ4QWJDNQ7-73874190-24</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAC4C16-FDF5-437E-A8C4-D650CA39502E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17639,7 +17649,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -17647,20 +17657,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding display name PP SKU Swatches Rolledup Count
</commit_message>
<xml_diff>
--- a/jcp-v4/99-exceldmd/Base Data Model.xlsx
+++ b/jcp-v4/99-exceldmd/Base Data Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/dataplatform-sampledata/jcp-v4/99-exceldmd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shyam.potta/rdp-sourcecode/dataplatform-sampledata/jcp-v4/99-exceldmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -45,8 +45,8 @@
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3368" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="967">
   <si>
     <t>ACTION</t>
   </si>
@@ -3038,6 +3038,9 @@
   </si>
   <si>
     <t>PRINT/PATTERN</t>
+  </si>
+  <si>
+    <t>PP SKU Swatches Rolledup Count</t>
   </si>
 </sst>
 </file>
@@ -3902,12 +3905,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
+      <selection activeCell="A5" sqref="A5"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
       <selection activeCell="B34" sqref="B34"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
-      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4079,11 +4082,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4159,14 +4162,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4180,10 +4183,10 @@
   <dimension ref="A1:AF255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9118,6 +9121,9 @@
       <c r="E163" t="s">
         <v>156</v>
       </c>
+      <c r="F163" t="s">
+        <v>966</v>
+      </c>
       <c r="G163" t="s">
         <v>42</v>
       </c>
@@ -11287,9 +11293,9 @@
   </sheetData>
   <autoFilter ref="A1:AE255"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11297,9 +11303,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11530,14 +11536,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -17044,12 +17050,6 @@
   </sheetData>
   <autoFilter ref="A1:AA475"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
-    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17060,6 +17060,12 @@
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D150">
@@ -17156,12 +17162,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17264,12 +17270,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17355,12 +17361,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>